<commit_message>
testes dia 15 de junho
</commit_message>
<xml_diff>
--- a/resultados/Tabela_Resultados_Validação.xlsx
+++ b/resultados/Tabela_Resultados_Validação.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\NotebooksMateriais\previsao_custo_salario_cestas\resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE21909-C6FE-49CA-8E57-0D9AF50D6963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A59BB8-7863-4138-BE46-E3EBC7D4F155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AC58E7D1-5F1F-4739-995F-1D0DCEA10BB9}"/>
   </bookViews>
@@ -191,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -205,45 +205,46 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,7 +562,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,314 +631,321 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="11">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11">
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7">
         <v>24</v>
       </c>
-      <c r="E2" s="11">
-        <v>3</v>
-      </c>
-      <c r="F2" s="12">
+      <c r="E2" s="7">
+        <v>3</v>
+      </c>
+      <c r="F2" s="8">
         <v>6361</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="9">
         <v>24</v>
       </c>
-      <c r="K2" s="15">
-        <v>1</v>
-      </c>
-      <c r="L2" s="15">
+      <c r="K2" s="9">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9">
         <v>25</v>
       </c>
-      <c r="M2" s="15">
-        <v>3</v>
-      </c>
-      <c r="N2" s="16">
+      <c r="M2" s="9">
+        <v>3</v>
+      </c>
+      <c r="N2" s="10">
         <v>5476</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11">
-        <v>32</v>
-      </c>
-      <c r="E3" s="11">
-        <v>3</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>32</v>
+      </c>
+      <c r="E3" s="7">
+        <v>3</v>
+      </c>
+      <c r="F3" s="8">
         <v>6018</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="15">
-        <v>32</v>
-      </c>
-      <c r="K3" s="15">
-        <v>1</v>
-      </c>
-      <c r="L3" s="15">
+      <c r="H3" s="16"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="9">
+        <v>32</v>
+      </c>
+      <c r="K3" s="9">
+        <v>1</v>
+      </c>
+      <c r="L3" s="9">
         <v>25</v>
       </c>
-      <c r="M3" s="15">
-        <v>3</v>
-      </c>
-      <c r="N3" s="16">
+      <c r="M3" s="9">
+        <v>3</v>
+      </c>
+      <c r="N3" s="10">
         <v>5268</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11">
-        <v>1</v>
-      </c>
-      <c r="D4" s="11">
-        <v>64</v>
-      </c>
-      <c r="E4" s="11">
-        <v>3</v>
-      </c>
-      <c r="F4" s="12">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>64</v>
+      </c>
+      <c r="E4" s="7">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8">
         <v>6754</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="15">
-        <v>64</v>
-      </c>
-      <c r="K4" s="15">
-        <v>1</v>
-      </c>
-      <c r="L4" s="15">
+      <c r="H4" s="16"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="9">
+        <v>64</v>
+      </c>
+      <c r="K4" s="9">
+        <v>1</v>
+      </c>
+      <c r="L4" s="9">
         <v>25</v>
       </c>
-      <c r="M4" s="15">
-        <v>3</v>
-      </c>
-      <c r="N4" s="16">
+      <c r="M4" s="9">
+        <v>3</v>
+      </c>
+      <c r="N4" s="10">
         <v>5037</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="11">
-        <v>1</v>
-      </c>
-      <c r="D5" s="11">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
         <v>24</v>
       </c>
-      <c r="E5" s="11">
-        <v>3</v>
-      </c>
-      <c r="F5" s="12">
+      <c r="E5" s="7">
+        <v>3</v>
+      </c>
+      <c r="F5" s="8">
         <v>5413</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="15">
+      <c r="H5" s="16"/>
+      <c r="I5" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="9">
         <v>24</v>
       </c>
-      <c r="K5" s="15">
-        <v>1</v>
-      </c>
-      <c r="L5" s="15">
+      <c r="K5" s="9">
+        <v>1</v>
+      </c>
+      <c r="L5" s="9">
         <v>25</v>
       </c>
-      <c r="M5" s="15">
-        <v>3</v>
-      </c>
-      <c r="N5" s="16">
+      <c r="M5" s="9">
+        <v>3</v>
+      </c>
+      <c r="N5" s="10">
         <v>5462</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11">
-        <v>1</v>
-      </c>
-      <c r="D6" s="11">
-        <v>32</v>
-      </c>
-      <c r="E6" s="11">
-        <v>3</v>
-      </c>
-      <c r="F6" s="12">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>32</v>
+      </c>
+      <c r="E6" s="7">
+        <v>3</v>
+      </c>
+      <c r="F6" s="8">
         <v>4976</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15">
-        <v>32</v>
-      </c>
-      <c r="K6" s="15">
-        <v>1</v>
-      </c>
-      <c r="L6" s="15">
+      <c r="H6" s="16"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="9">
+        <v>32</v>
+      </c>
+      <c r="K6" s="9">
+        <v>1</v>
+      </c>
+      <c r="L6" s="9">
         <v>25</v>
       </c>
-      <c r="M6" s="15">
-        <v>3</v>
-      </c>
-      <c r="N6" s="16">
+      <c r="M6" s="9">
+        <v>3</v>
+      </c>
+      <c r="N6" s="10">
         <v>5414</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11">
-        <v>64</v>
-      </c>
-      <c r="E7" s="11">
-        <v>3</v>
-      </c>
-      <c r="F7" s="12">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>64</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="8">
         <v>4697</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15">
-        <v>64</v>
-      </c>
-      <c r="K7" s="15">
-        <v>1</v>
-      </c>
-      <c r="L7" s="15">
+      <c r="H7" s="16"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="9">
+        <v>64</v>
+      </c>
+      <c r="K7" s="9">
+        <v>1</v>
+      </c>
+      <c r="L7" s="9">
         <v>25</v>
       </c>
-      <c r="M7" s="15">
-        <v>3</v>
-      </c>
-      <c r="N7" s="16">
+      <c r="M7" s="9">
+        <v>3</v>
+      </c>
+      <c r="N7" s="10">
         <v>5032</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="8">
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
         <v>24</v>
       </c>
-      <c r="E8" s="8">
-        <v>3</v>
-      </c>
-      <c r="F8" s="9">
+      <c r="E8" s="5">
+        <v>3</v>
+      </c>
+      <c r="F8" s="6">
         <v>5716</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8">
-        <v>1</v>
-      </c>
-      <c r="D9" s="8">
-        <v>32</v>
-      </c>
-      <c r="E9" s="8">
-        <v>3</v>
-      </c>
-      <c r="F9" s="9">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>32</v>
+      </c>
+      <c r="E9" s="5">
+        <v>3</v>
+      </c>
+      <c r="F9" s="6">
         <v>5778</v>
       </c>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8">
-        <v>1</v>
-      </c>
-      <c r="D10" s="8">
-        <v>64</v>
-      </c>
-      <c r="E10" s="8">
-        <v>3</v>
-      </c>
-      <c r="F10" s="9">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <v>64</v>
+      </c>
+      <c r="E10" s="5">
+        <v>3</v>
+      </c>
+      <c r="F10" s="6">
         <v>5635</v>
       </c>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="8">
-        <v>1</v>
-      </c>
-      <c r="D11" s="8">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
         <v>24</v>
       </c>
-      <c r="E11" s="8">
-        <v>3</v>
-      </c>
-      <c r="F11" s="9">
+      <c r="E11" s="5">
+        <v>3</v>
+      </c>
+      <c r="F11" s="6">
         <v>5644</v>
       </c>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8">
-        <v>1</v>
-      </c>
-      <c r="D12" s="8">
-        <v>32</v>
-      </c>
-      <c r="E12" s="8">
-        <v>3</v>
-      </c>
-      <c r="F12" s="9" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5">
+        <v>32</v>
+      </c>
+      <c r="E12" s="5">
+        <v>3</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8">
-        <v>1</v>
-      </c>
-      <c r="D13" s="8">
-        <v>64</v>
-      </c>
-      <c r="E13" s="8">
-        <v>3</v>
-      </c>
-      <c r="F13" s="9">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5">
+        <v>64</v>
+      </c>
+      <c r="E13" s="5">
+        <v>3</v>
+      </c>
+      <c r="F13" s="6">
         <v>5488</v>
       </c>
     </row>
@@ -965,247 +973,253 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="11">
-        <v>2</v>
-      </c>
-      <c r="D16" s="11">
-        <v>32</v>
-      </c>
-      <c r="E16" s="11">
+      <c r="C16" s="7">
+        <v>2</v>
+      </c>
+      <c r="D16" s="7">
+        <v>32</v>
+      </c>
+      <c r="E16" s="7">
         <v>16</v>
       </c>
-      <c r="F16" s="11">
-        <v>3</v>
-      </c>
-      <c r="G16" s="12">
+      <c r="F16" s="7">
+        <v>3</v>
+      </c>
+      <c r="G16" s="8">
         <v>7302</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11">
-        <v>2</v>
-      </c>
-      <c r="D17" s="11">
-        <v>32</v>
-      </c>
-      <c r="E17" s="11">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="7">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7">
+        <v>32</v>
+      </c>
+      <c r="E17" s="7">
         <v>24</v>
       </c>
-      <c r="F17" s="11">
-        <v>3</v>
-      </c>
-      <c r="G17" s="12">
+      <c r="F17" s="7">
+        <v>3</v>
+      </c>
+      <c r="G17" s="8">
         <v>7097</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11">
-        <v>2</v>
-      </c>
-      <c r="D18" s="11">
-        <v>32</v>
-      </c>
-      <c r="E18" s="11">
-        <v>32</v>
-      </c>
-      <c r="F18" s="11">
-        <v>3</v>
-      </c>
-      <c r="G18" s="12">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="7">
+        <v>2</v>
+      </c>
+      <c r="D18" s="7">
+        <v>32</v>
+      </c>
+      <c r="E18" s="7">
+        <v>32</v>
+      </c>
+      <c r="F18" s="7">
+        <v>3</v>
+      </c>
+      <c r="G18" s="8">
         <v>7651</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="11">
-        <v>2</v>
-      </c>
-      <c r="D19" s="11">
-        <v>32</v>
-      </c>
-      <c r="E19" s="11">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2</v>
+      </c>
+      <c r="D19" s="7">
+        <v>32</v>
+      </c>
+      <c r="E19" s="7">
         <v>16</v>
       </c>
-      <c r="F19" s="11">
-        <v>3</v>
-      </c>
-      <c r="G19" s="12">
+      <c r="F19" s="7">
+        <v>3</v>
+      </c>
+      <c r="G19" s="8">
         <v>5358</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11">
-        <v>2</v>
-      </c>
-      <c r="D20" s="11">
-        <v>32</v>
-      </c>
-      <c r="E20" s="11">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="7">
+        <v>2</v>
+      </c>
+      <c r="D20" s="7">
+        <v>32</v>
+      </c>
+      <c r="E20" s="7">
         <v>24</v>
       </c>
-      <c r="F20" s="11">
-        <v>3</v>
-      </c>
-      <c r="G20" s="12">
+      <c r="F20" s="7">
+        <v>3</v>
+      </c>
+      <c r="G20" s="8">
         <v>4846</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11">
-        <v>2</v>
-      </c>
-      <c r="D21" s="11">
-        <v>32</v>
-      </c>
-      <c r="E21" s="11">
-        <v>32</v>
-      </c>
-      <c r="F21" s="11">
-        <v>3</v>
-      </c>
-      <c r="G21" s="12">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="7">
+        <v>2</v>
+      </c>
+      <c r="D21" s="7">
+        <v>32</v>
+      </c>
+      <c r="E21" s="7">
+        <v>32</v>
+      </c>
+      <c r="F21" s="7">
+        <v>3</v>
+      </c>
+      <c r="G21" s="8">
         <v>4798</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="8">
-        <v>2</v>
-      </c>
-      <c r="D22" s="8">
-        <v>64</v>
-      </c>
-      <c r="E22" s="8">
+      <c r="C22" s="5">
+        <v>2</v>
+      </c>
+      <c r="D22" s="5">
+        <v>64</v>
+      </c>
+      <c r="E22" s="5">
         <v>24</v>
       </c>
-      <c r="F22" s="8">
-        <v>3</v>
-      </c>
-      <c r="G22" s="9">
+      <c r="F22" s="5">
+        <v>3</v>
+      </c>
+      <c r="G22" s="6">
         <v>5864</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8">
-        <v>2</v>
-      </c>
-      <c r="D23" s="8">
-        <v>64</v>
-      </c>
-      <c r="E23" s="8">
-        <v>32</v>
-      </c>
-      <c r="F23" s="8">
-        <v>3</v>
-      </c>
-      <c r="G23" s="9">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="5">
+        <v>2</v>
+      </c>
+      <c r="D23" s="5">
+        <v>64</v>
+      </c>
+      <c r="E23" s="5">
+        <v>32</v>
+      </c>
+      <c r="F23" s="5">
+        <v>3</v>
+      </c>
+      <c r="G23" s="6">
         <v>5723</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8">
-        <v>2</v>
-      </c>
-      <c r="D24" s="8">
-        <v>64</v>
-      </c>
-      <c r="E24" s="8">
-        <v>64</v>
-      </c>
-      <c r="F24" s="8">
-        <v>3</v>
-      </c>
-      <c r="G24" s="9">
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="5">
+        <v>2</v>
+      </c>
+      <c r="D24" s="5">
+        <v>64</v>
+      </c>
+      <c r="E24" s="5">
+        <v>64</v>
+      </c>
+      <c r="F24" s="5">
+        <v>3</v>
+      </c>
+      <c r="G24" s="6">
         <v>5747</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="8">
-        <v>2</v>
-      </c>
-      <c r="D25" s="8">
-        <v>64</v>
-      </c>
-      <c r="E25" s="8">
+      <c r="A25" s="12"/>
+      <c r="B25" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="5">
+        <v>2</v>
+      </c>
+      <c r="D25" s="5">
+        <v>64</v>
+      </c>
+      <c r="E25" s="5">
         <v>24</v>
       </c>
-      <c r="F25" s="8">
-        <v>3</v>
-      </c>
-      <c r="G25" s="9">
+      <c r="F25" s="5">
+        <v>3</v>
+      </c>
+      <c r="G25" s="6">
         <v>5600</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="8">
-        <v>2</v>
-      </c>
-      <c r="D26" s="8">
-        <v>64</v>
-      </c>
-      <c r="E26" s="8">
-        <v>32</v>
-      </c>
-      <c r="F26" s="8">
-        <v>3</v>
-      </c>
-      <c r="G26" s="9">
+      <c r="A26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="5">
+        <v>2</v>
+      </c>
+      <c r="D26" s="5">
+        <v>64</v>
+      </c>
+      <c r="E26" s="5">
+        <v>32</v>
+      </c>
+      <c r="F26" s="5">
+        <v>3</v>
+      </c>
+      <c r="G26" s="6">
         <v>5585</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8">
-        <v>2</v>
-      </c>
-      <c r="D27" s="8">
-        <v>64</v>
-      </c>
-      <c r="E27" s="8">
-        <v>64</v>
-      </c>
-      <c r="F27" s="8">
-        <v>3</v>
-      </c>
-      <c r="G27" s="17">
+      <c r="A27" s="12"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="5">
+        <v>2</v>
+      </c>
+      <c r="D27" s="5">
+        <v>64</v>
+      </c>
+      <c r="E27" s="5">
+        <v>64</v>
+      </c>
+      <c r="F27" s="5">
+        <v>3</v>
+      </c>
+      <c r="G27" s="11">
         <v>5570</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
     <mergeCell ref="A22:A27"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B25:B27"/>
@@ -1215,12 +1229,6 @@
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B11:B13"/>
-    <mergeCell ref="H2:H7"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B21"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>